<commit_message>
corrected .v files, added report and groupmembers.xlsx
</commit_message>
<xml_diff>
--- a/GroupMembers.xlsx
+++ b/GroupMembers.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8933E6A7-E95B-467B-B1A5-D78E58A3E452}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B2E726-EBC6-4C33-A58B-38B2D32DB86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>CRN</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>StudentID</t>
+  </si>
+  <si>
+    <t>Alperen Akbaş</t>
+  </si>
+  <si>
+    <t>Ömer Faruk Ekmekçi</t>
   </si>
 </sst>
 </file>
@@ -346,20 +352,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,9 +374,32 @@
       </c>
       <c r="C1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>22599</v>
+      </c>
+      <c r="B2">
+        <v>150220078</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>22599</v>
+      </c>
+      <c r="B3">
+        <v>150230046</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>